<commit_message>
updated CP to have equal wieghts for each habitat and the flower plot display and documentation
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="0" windowWidth="25600" windowHeight="16600" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="1740" yWindow="0" windowWidth="25600" windowHeight="16560" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4087" uniqueCount="2031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4090" uniqueCount="2033">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9182,6 +9182,12 @@
   </si>
   <si>
     <t>removed carbon storage goal - Hawaii Island got a bad score unfairly if it was included - a small amount of wetland/saltmarsh area and it was lost</t>
+  </si>
+  <si>
+    <t>remove extent as weight on final scores - this reduced the scores to just an average of the condition s of each habitat  - should be set a reference for wetland health at 50% of historical wetlands intact? This would raise the scores a bit.</t>
+  </si>
+  <si>
+    <t>fishpond helath information is needed if we are not including extent data in this assessment</t>
   </si>
 </sst>
 </file>
@@ -13096,10 +13102,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14345,7 +14351,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="30">
+    <row r="113" spans="1:4" ht="30">
       <c r="A113" s="140">
         <v>42978</v>
       </c>
@@ -14354,6 +14360,20 @@
       </c>
       <c r="C113" s="28" t="s">
         <v>2030</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="30">
+      <c r="A114" s="140">
+        <v>42979</v>
+      </c>
+      <c r="B114" t="s">
+        <v>731</v>
+      </c>
+      <c r="C114" s="28" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D114" t="s">
+        <v>2032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating pressure layers associated with tourism and marine debris
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35660" yWindow="-1480" windowWidth="32640" windowHeight="17460" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4355" uniqueCount="2128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4369" uniqueCount="2138">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9483,6 +9483,36 @@
   </si>
   <si>
     <t>Information Technology &amp; Innovation Foundation</t>
+  </si>
+  <si>
+    <t>11/14/17-12/5/17</t>
+  </si>
+  <si>
+    <t>website updates, all data layers displayed on web and all goal descriptions from using Data_layers file in prep folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presented WH OHI at the NOAA IEA workshop </t>
+  </si>
+  <si>
+    <t>12/18/17</t>
+  </si>
+  <si>
+    <t>met with Joey Lecky to review and update pressure layers used in both the MHI and WH OHI</t>
+  </si>
+  <si>
+    <t>12/21/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated marine debris pressure using Moy et al 2017 table 3. reference is the % county # of marine debris counts to the state counts. Niihoa is the highest - so rgn_4 is the highest </t>
+  </si>
+  <si>
+    <t>pressures</t>
+  </si>
+  <si>
+    <t>tourism - calculated from HTA visitor participation surveys and multipled by the number of visitors (2015) by county to get # of participants per ocean activity and referenced to the regional maximum per activity; (Oahu in all cases); added each activiity as separate tourism pressure layer</t>
+  </si>
+  <si>
+    <t>added all the t_ pressure layers to the pressures matrix, categories, and layers.csv</t>
   </si>
 </sst>
 </file>
@@ -13531,10 +13561,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14987,6 +15017,63 @@
       </c>
       <c r="C131" s="28" t="s">
         <v>1957</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>2128</v>
+      </c>
+      <c r="C132" s="28" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="140">
+        <v>42898</v>
+      </c>
+      <c r="C133" s="28" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C135" s="28" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C136" s="28" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C137" s="28" t="s">
+        <v>2137</v>
       </c>
     </row>
   </sheetData>
@@ -15006,7 +15093,7 @@
   </sheetPr>
   <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>

</xml_diff>

<commit_message>
updated FIS, removed coastal pelagics from reef fish tables, layers, and scores and moved to thier own layer and tables
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35900" yWindow="2320" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="-33780" yWindow="160" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -13628,7 +13628,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated FIS and datalayers with the 2018 bottom fish stock assessment
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="2189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4442" uniqueCount="2190">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9666,6 +9666,9 @@
   </si>
   <si>
     <t>removed access from AO and changed name to nearshore fisheries</t>
+  </si>
+  <si>
+    <t>updated fish_sus_updated_mhi2017 with new bottomfish stock assessment scores, used linear regression for past ten years of data to predict 2016 b/bmsy score</t>
   </si>
 </sst>
 </file>
@@ -13733,10 +13736,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -15523,6 +15526,17 @@
       </c>
       <c r="C162" s="28" t="s">
         <v>2188</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="32">
+      <c r="A163" s="140">
+        <v>43300</v>
+      </c>
+      <c r="B163" t="s">
+        <v>690</v>
+      </c>
+      <c r="C163" s="28" t="s">
+        <v>2189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created resilience layer on shoreline access
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4442" uniqueCount="2190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4444" uniqueCount="2191">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9669,6 +9669,9 @@
   </si>
   <si>
     <t>updated fish_sus_updated_mhi2017 with new bottomfish stock assessment scores, used linear regression for past ten years of data to predict 2016 b/bmsy score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on access layer - is it a pressure or resilience layer or part of nearshore fisheries indicator </t>
   </si>
 </sst>
 </file>
@@ -13736,10 +13739,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -15537,6 +15540,17 @@
       </c>
       <c r="C163" s="28" t="s">
         <v>2189</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="140">
+        <v>43300</v>
+      </c>
+      <c r="B164" t="s">
+        <v>690</v>
+      </c>
+      <c r="C164" s="28" t="s">
+        <v>2190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added access as a resilience layer for nearshore fisheries and reran scores
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31280" yWindow="-920" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="540" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4444" uniqueCount="2191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4447" uniqueCount="2194">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9672,6 +9672,15 @@
   </si>
   <si>
     <t xml:space="preserve">working on access layer - is it a pressure or resilience layer or part of nearshore fisheries indicator </t>
+  </si>
+  <si>
+    <t>DAR/ 30 by 30 integration and messaging meeting with Anne Chung, Kim Hum, Kristen Maize, Mary Donovan - working to integrate indicators and have consistent messaging. Removing the SP goal and putting recreation back in to the index</t>
+  </si>
+  <si>
+    <t>beach - metrics being developed in terms of % of coastline that is armored or developed with Joey lecky to be able to update in the future</t>
+  </si>
+  <si>
+    <t>meeting with HIMARC and 30 by 30. Indicator development - will follow up with DAR on OHI integration and messaging</t>
   </si>
 </sst>
 </file>
@@ -13739,10 +13748,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -15551,6 +15560,30 @@
       </c>
       <c r="C164" s="28" t="s">
         <v>2190</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="32">
+      <c r="A165" s="140">
+        <v>43301</v>
+      </c>
+      <c r="C165" s="28" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="140">
+        <v>44398</v>
+      </c>
+      <c r="C166" s="28" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="140">
+        <v>43302</v>
+      </c>
+      <c r="C167" s="28" t="s">
+        <v>2193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ST time series to 2016 and adding in daily visitor spending as indicator in economic indicators
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4447" uniqueCount="2194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="2195">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9681,6 +9681,9 @@
   </si>
   <si>
     <t>meeting with HIMARC and 30 by 30. Indicator development - will follow up with DAR on OHI integration and messaging</t>
+  </si>
+  <si>
+    <t>updated ST goal with 2016 data and added visitor spending per day to growth indicator (now an average of visitor expenditures and ddaily visitor spending)</t>
   </si>
 </sst>
 </file>
@@ -13748,10 +13751,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -15584,6 +15587,14 @@
       </c>
       <c r="C167" s="28" t="s">
         <v>2193</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="32">
+      <c r="A168" s="140">
+        <v>43303</v>
+      </c>
+      <c r="C168" s="28" t="s">
+        <v>2194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed spelling in website goal pages
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33760" yWindow="-580" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33120" yWindow="-1380" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4458" uniqueCount="2202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="2205">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9705,6 +9705,15 @@
   </si>
   <si>
     <t>created a new alternative layer on cp_hab_conidition_mhi2017 called cp_hab_condition_updated_mhi2017. We can choose which wetland data we want to use. The updated data layer uses percent of 1992 NOAA CCAP wetlands within 1 km of the shoreline. If we use this data set we can update the data every 5 years with NOAA CCAP data. The prior layer used topographic wetness analysis to estimate the percent of current wetlands to wetlands pre human contact.</t>
+  </si>
+  <si>
+    <t>wetlands alternate layer added for CP but not HAB based on NOAA CCAP 1992 extent. The change in resolution likely impacted the area estimates (over estimating in 1992) so the scores are going to be biased to lower values - this may be the case for Hawaii Island were the wetland cover is so low.</t>
+  </si>
+  <si>
+    <t>MAR/CP</t>
+  </si>
+  <si>
+    <t>sent email to Nakoa and Brenda about the fishpond metrics for review and update</t>
   </si>
 </sst>
 </file>
@@ -13772,10 +13781,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -15676,6 +15685,28 @@
       </c>
       <c r="C174" s="28" t="s">
         <v>2201</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="48">
+      <c r="A175" s="140">
+        <v>43192</v>
+      </c>
+      <c r="B175" t="s">
+        <v>919</v>
+      </c>
+      <c r="C175" s="28" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="140">
+        <v>43193</v>
+      </c>
+      <c r="B176" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C176" s="28" t="s">
+        <v>2204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated offshore fisheries and scores
</commit_message>
<xml_diff>
--- a/prep/OHI_state assessment_framework.xlsx
+++ b/prep/OHI_state assessment_framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33120" yWindow="-1380" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33840" yWindow="-2360" windowWidth="28800" windowHeight="17460" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OHI Hawaii Goals" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="2205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4464" uniqueCount="2206">
   <si>
     <t>30% of marine and terrestrial areas protected</t>
   </si>
@@ -9713,7 +9713,10 @@
     <t>MAR/CP</t>
   </si>
   <si>
-    <t>sent email to Nakoa and Brenda about the fishpond metrics for review and update</t>
+    <t>sent email to Nakoa and Brenda about the fishpond metrics for review and update - updated fishpond layer data will be available by the end of the week and we will meet to discuss metric</t>
+  </si>
+  <si>
+    <t>updated offshore fisheries with new stock assessment reports and updated goal score, sent to PIRO stock assessment division for review</t>
   </si>
 </sst>
 </file>
@@ -10614,7 +10617,7 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="518">
+  <cellXfs count="520">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -12035,6 +12038,10 @@
     <xf numFmtId="0" fontId="65" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="84">
     <cellStyle name="Bold text" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -13781,10 +13788,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -13792,6 +13799,7 @@
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="119" style="28" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -15698,7 +15706,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" ht="32">
       <c r="A176" s="140">
         <v>43193</v>
       </c>
@@ -15708,6 +15716,24 @@
       <c r="C176" s="28" t="s">
         <v>2204</v>
       </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="140">
+        <v>43194</v>
+      </c>
+      <c r="B177" t="s">
+        <v>690</v>
+      </c>
+      <c r="C177" s="28" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="D179" s="519"/>
+      <c r="E179" s="518"/>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="D180" s="519"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>